<commit_message>
ordination scaling issue update
</commit_message>
<xml_diff>
--- a/table/rda/biomass_rda_anova.xlsx
+++ b/table/rda/biomass_rda_anova.xlsx
@@ -361,7 +361,7 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>rownames(biomass_rda_axis)</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -528,7 +528,7 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>rownames(biomass_rda_margin)</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">

</xml_diff>